<commit_message>
Fixed excel and csv files
</commit_message>
<xml_diff>
--- a/sample.data.xlsx
+++ b/sample.data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aportugu/Desktop/Rworkshop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9A8408-E79C-1942-B541-C650B8C59683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA3C5352-1407-D447-8C02-B757FC1B9534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1394,8 +1394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DM130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BY102" workbookViewId="0">
-      <selection activeCell="CO133" sqref="CO133"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1782,7 +1782,7 @@
         <v>116</v>
       </c>
       <c r="J2">
-        <v>73.704109590000002</v>
+        <v>73.7</v>
       </c>
       <c r="K2">
         <v>27</v>
@@ -2099,7 +2099,7 @@
         <v>116</v>
       </c>
       <c r="J3">
-        <v>62.498630140000003</v>
+        <v>62.4</v>
       </c>
       <c r="K3">
         <v>27</v>
@@ -2392,7 +2392,7 @@
         <v>116</v>
       </c>
       <c r="J4">
-        <v>50.265753420000003</v>
+        <v>50.2</v>
       </c>
       <c r="K4">
         <v>28</v>
@@ -2676,7 +2676,7 @@
         <v>116</v>
       </c>
       <c r="J5">
-        <v>33.665753420000001</v>
+        <v>33.6</v>
       </c>
       <c r="K5">
         <v>28</v>
@@ -2966,7 +2966,7 @@
         <v>116</v>
       </c>
       <c r="J6">
-        <v>55.94794521</v>
+        <v>55.9</v>
       </c>
       <c r="K6">
         <v>33</v>
@@ -3244,7 +3244,7 @@
         <v>116</v>
       </c>
       <c r="J7">
-        <v>53.145205480000001</v>
+        <v>53.1</v>
       </c>
       <c r="K7">
         <v>23</v>
@@ -3549,7 +3549,7 @@
         <v>116</v>
       </c>
       <c r="J8">
-        <v>67.931506850000005</v>
+        <v>67.900000000000006</v>
       </c>
       <c r="K8">
         <v>21</v>
@@ -3860,7 +3860,7 @@
         <v>116</v>
       </c>
       <c r="J9">
-        <v>33.550684930000003</v>
+        <v>33.5</v>
       </c>
       <c r="K9">
         <v>30</v>
@@ -4141,7 +4141,7 @@
         <v>116</v>
       </c>
       <c r="J10">
-        <v>42.435616439999997</v>
+        <v>42.4</v>
       </c>
       <c r="K10">
         <v>26</v>
@@ -4446,7 +4446,7 @@
         <v>116</v>
       </c>
       <c r="J11">
-        <v>67.564383559999996</v>
+        <v>67.5</v>
       </c>
       <c r="K11">
         <v>40</v>
@@ -4763,7 +4763,7 @@
         <v>116</v>
       </c>
       <c r="J12">
-        <v>68.241095889999997</v>
+        <v>68.2</v>
       </c>
       <c r="K12">
         <v>41</v>
@@ -5101,7 +5101,7 @@
         <v>116</v>
       </c>
       <c r="J13">
-        <v>70.07945205</v>
+        <v>70</v>
       </c>
       <c r="K13">
         <v>27</v>
@@ -5439,7 +5439,7 @@
         <v>130</v>
       </c>
       <c r="J14">
-        <v>65.742465749999994</v>
+        <v>65.7</v>
       </c>
       <c r="K14">
         <v>91</v>
@@ -5762,7 +5762,7 @@
         <v>130</v>
       </c>
       <c r="J15">
-        <v>77.18082192</v>
+        <v>77.099999999999994</v>
       </c>
       <c r="K15">
         <v>30</v>
@@ -6061,7 +6061,7 @@
         <v>116</v>
       </c>
       <c r="J16">
-        <v>65.838356160000004</v>
+        <v>65.8</v>
       </c>
       <c r="K16">
         <v>26</v>
@@ -6375,7 +6375,7 @@
         <v>130</v>
       </c>
       <c r="J17">
-        <v>66.53150685</v>
+        <v>66.5</v>
       </c>
       <c r="K17">
         <v>30</v>
@@ -6716,7 +6716,7 @@
         <v>116</v>
       </c>
       <c r="J18">
-        <v>73.663013699999993</v>
+        <v>73.599999999999994</v>
       </c>
       <c r="K18">
         <v>28</v>
@@ -7021,7 +7021,7 @@
         <v>130</v>
       </c>
       <c r="J19">
-        <v>55.630136989999997</v>
+        <v>55.6</v>
       </c>
       <c r="K19">
         <v>29</v>
@@ -7365,7 +7365,7 @@
         <v>130</v>
       </c>
       <c r="J20">
-        <v>74.816438360000006</v>
+        <v>74.8</v>
       </c>
       <c r="K20">
         <v>31</v>
@@ -7679,7 +7679,7 @@
         <v>116</v>
       </c>
       <c r="J21">
-        <v>67.153424659999999</v>
+        <v>67.099999999999994</v>
       </c>
       <c r="K21">
         <v>27</v>
@@ -8011,7 +8011,7 @@
         <v>116</v>
       </c>
       <c r="J22">
-        <v>61.276712330000002</v>
+        <v>61.2</v>
       </c>
       <c r="K22">
         <v>23</v>
@@ -8343,7 +8343,7 @@
         <v>130</v>
       </c>
       <c r="J23">
-        <v>68.835616439999995</v>
+        <v>68.8</v>
       </c>
       <c r="K23">
         <v>39</v>
@@ -8645,7 +8645,7 @@
         <v>130</v>
       </c>
       <c r="J24">
-        <v>77.205479449999999</v>
+        <v>77.2</v>
       </c>
       <c r="K24">
         <v>30</v>
@@ -8959,7 +8959,7 @@
         <v>130</v>
       </c>
       <c r="J25">
-        <v>54.583561639999999</v>
+        <v>54.5</v>
       </c>
       <c r="K25">
         <v>31</v>
@@ -9306,7 +9306,7 @@
         <v>130</v>
       </c>
       <c r="J26">
-        <v>62.567123289999998</v>
+        <v>62.5</v>
       </c>
       <c r="K26">
         <v>33</v>
@@ -9605,7 +9605,7 @@
         <v>116</v>
       </c>
       <c r="J27">
-        <v>70.386301369999998</v>
+        <v>70.3</v>
       </c>
       <c r="K27">
         <v>26</v>
@@ -9904,7 +9904,7 @@
         <v>130</v>
       </c>
       <c r="J28">
-        <v>47.282191779999998</v>
+        <v>47.2</v>
       </c>
       <c r="K28">
         <v>32</v>
@@ -10200,7 +10200,7 @@
         <v>130</v>
       </c>
       <c r="J29">
-        <v>83.282191780000005</v>
+        <v>83.2</v>
       </c>
       <c r="K29">
         <v>30</v>
@@ -10514,7 +10514,7 @@
         <v>130</v>
       </c>
       <c r="J30">
-        <v>61.882191779999999</v>
+        <v>61.8</v>
       </c>
       <c r="K30">
         <v>35</v>
@@ -10813,7 +10813,7 @@
         <v>130</v>
       </c>
       <c r="J31">
-        <v>71.002739730000002</v>
+        <v>71</v>
       </c>
       <c r="K31">
         <v>36</v>
@@ -11133,7 +11133,7 @@
         <v>130</v>
       </c>
       <c r="J32">
-        <v>65.479452050000006</v>
+        <v>65.400000000000006</v>
       </c>
       <c r="K32">
         <v>40</v>
@@ -11432,7 +11432,7 @@
         <v>130</v>
       </c>
       <c r="J33">
-        <v>67.632876710000005</v>
+        <v>67.599999999999994</v>
       </c>
       <c r="K33">
         <v>36</v>
@@ -11713,7 +11713,7 @@
         <v>130</v>
       </c>
       <c r="J34">
-        <v>76.405479450000001</v>
+        <v>76.400000000000006</v>
       </c>
       <c r="K34">
         <v>31</v>
@@ -12051,7 +12051,7 @@
         <v>130</v>
       </c>
       <c r="J35">
-        <v>71.775342469999998</v>
+        <v>71.7</v>
       </c>
       <c r="K35">
         <v>28</v>
@@ -12362,7 +12362,7 @@
         <v>130</v>
       </c>
       <c r="J36">
-        <v>72.578082190000003</v>
+        <v>72.5</v>
       </c>
       <c r="K36">
         <v>56</v>
@@ -12646,7 +12646,7 @@
         <v>130</v>
       </c>
       <c r="J37">
-        <v>76.479452050000006</v>
+        <v>76.400000000000006</v>
       </c>
       <c r="K37">
         <v>39</v>
@@ -12945,7 +12945,7 @@
         <v>130</v>
       </c>
       <c r="J38">
-        <v>68.347945210000006</v>
+        <v>68.3</v>
       </c>
       <c r="K38">
         <v>34</v>
@@ -13289,7 +13289,7 @@
         <v>130</v>
       </c>
       <c r="J39">
-        <v>74.542465750000005</v>
+        <v>74.5</v>
       </c>
       <c r="K39">
         <v>44</v>
@@ -13579,7 +13579,7 @@
         <v>130</v>
       </c>
       <c r="J40">
-        <v>63.964383560000002</v>
+        <v>63.9</v>
       </c>
       <c r="K40">
         <v>32</v>
@@ -13884,7 +13884,7 @@
         <v>130</v>
       </c>
       <c r="J41">
-        <v>58.821917810000002</v>
+        <v>58.8</v>
       </c>
       <c r="K41">
         <v>49</v>
@@ -14180,7 +14180,7 @@
         <v>130</v>
       </c>
       <c r="J42">
-        <v>79.81917808</v>
+        <v>79.8</v>
       </c>
       <c r="K42">
         <v>38</v>
@@ -14485,7 +14485,7 @@
         <v>130</v>
       </c>
       <c r="J43">
-        <v>56.331506849999997</v>
+        <v>56.3</v>
       </c>
       <c r="K43">
         <v>48</v>
@@ -14784,7 +14784,7 @@
         <v>130</v>
       </c>
       <c r="J44">
-        <v>75.536986299999995</v>
+        <v>75.5</v>
       </c>
       <c r="K44">
         <v>35</v>
@@ -15113,7 +15113,7 @@
         <v>116</v>
       </c>
       <c r="J45">
-        <v>42.241095889999997</v>
+        <v>42.2</v>
       </c>
       <c r="K45">
         <v>26</v>
@@ -15442,7 +15442,7 @@
         <v>116</v>
       </c>
       <c r="J46">
-        <v>66.115068489999999</v>
+        <v>66.099999999999994</v>
       </c>
       <c r="K46">
         <v>27</v>
@@ -15750,7 +15750,7 @@
         <v>116</v>
       </c>
       <c r="J47">
-        <v>62.117808220000001</v>
+        <v>62.1</v>
       </c>
       <c r="K47">
         <v>47</v>
@@ -16088,7 +16088,7 @@
         <v>116</v>
       </c>
       <c r="J48">
-        <v>50.854794519999999</v>
+        <v>50.8</v>
       </c>
       <c r="K48">
         <v>62</v>
@@ -16414,7 +16414,7 @@
         <v>130</v>
       </c>
       <c r="J49">
-        <v>67.183561639999994</v>
+        <v>67.099999999999994</v>
       </c>
       <c r="K49">
         <v>32</v>
@@ -16740,7 +16740,7 @@
         <v>130</v>
       </c>
       <c r="J50">
-        <v>75.134246579999996</v>
+        <v>75.099999999999994</v>
       </c>
       <c r="K50">
         <v>53</v>
@@ -17069,7 +17069,7 @@
         <v>130</v>
       </c>
       <c r="J51">
-        <v>66.761643840000005</v>
+        <v>66.7</v>
       </c>
       <c r="K51">
         <v>32</v>
@@ -17383,7 +17383,7 @@
         <v>130</v>
       </c>
       <c r="J52">
-        <v>72.55890411</v>
+        <v>72.5</v>
       </c>
       <c r="K52">
         <v>42</v>
@@ -17691,7 +17691,7 @@
         <v>130</v>
       </c>
       <c r="J53">
-        <v>48.123287670000003</v>
+        <v>48.1</v>
       </c>
       <c r="K53">
         <v>33</v>
@@ -18002,7 +18002,7 @@
         <v>116</v>
       </c>
       <c r="J54">
-        <v>52.632876709999998</v>
+        <v>52.6</v>
       </c>
       <c r="K54">
         <v>24</v>
@@ -18334,7 +18334,7 @@
         <v>130</v>
       </c>
       <c r="J55">
-        <v>72.019178080000003</v>
+        <v>72</v>
       </c>
       <c r="K55">
         <v>49</v>
@@ -18627,7 +18627,7 @@
         <v>116</v>
       </c>
       <c r="J56">
-        <v>26.476712330000002</v>
+        <v>26.4</v>
       </c>
       <c r="K56">
         <v>28</v>
@@ -18923,7 +18923,7 @@
         <v>116</v>
       </c>
       <c r="J57">
-        <v>64.553424660000005</v>
+        <v>64.5</v>
       </c>
       <c r="K57">
         <v>26</v>
@@ -19252,7 +19252,7 @@
         <v>130</v>
       </c>
       <c r="J58">
-        <v>59.446575340000003</v>
+        <v>59.4</v>
       </c>
       <c r="K58">
         <v>33</v>
@@ -19590,7 +19590,7 @@
         <v>130</v>
       </c>
       <c r="J59">
-        <v>55.71506849</v>
+        <v>55.7</v>
       </c>
       <c r="K59">
         <v>43</v>
@@ -19880,7 +19880,7 @@
         <v>116</v>
       </c>
       <c r="J60">
-        <v>54.616438359999997</v>
+        <v>54.6</v>
       </c>
       <c r="K60">
         <v>33</v>
@@ -20227,7 +20227,7 @@
         <v>130</v>
       </c>
       <c r="J61">
-        <v>64.44109589</v>
+        <v>64.400000000000006</v>
       </c>
       <c r="K61">
         <v>41</v>
@@ -20565,7 +20565,7 @@
         <v>130</v>
       </c>
       <c r="J62">
-        <v>54.704109590000002</v>
+        <v>54.7</v>
       </c>
       <c r="K62">
         <v>53</v>
@@ -20858,7 +20858,7 @@
         <v>130</v>
       </c>
       <c r="J63">
-        <v>55.983561639999998</v>
+        <v>55.9</v>
       </c>
       <c r="K63">
         <v>34</v>
@@ -21145,7 +21145,7 @@
         <v>130</v>
       </c>
       <c r="J64">
-        <v>41.446575340000003</v>
+        <v>41.4</v>
       </c>
       <c r="K64">
         <v>40</v>
@@ -21441,7 +21441,7 @@
         <v>130</v>
       </c>
       <c r="J65">
-        <v>68.287671230000001</v>
+        <v>68.2</v>
       </c>
       <c r="K65">
         <v>35</v>
@@ -21740,7 +21740,7 @@
         <v>130</v>
       </c>
       <c r="J66">
-        <v>76.175342470000004</v>
+        <v>76.099999999999994</v>
       </c>
       <c r="K66">
         <v>33</v>
@@ -22033,7 +22033,7 @@
         <v>116</v>
       </c>
       <c r="J67">
-        <v>73.476712329999998</v>
+        <v>73.400000000000006</v>
       </c>
       <c r="K67">
         <v>38</v>
@@ -22329,7 +22329,7 @@
         <v>130</v>
       </c>
       <c r="J68">
-        <v>44.997260269999998</v>
+        <v>44.9</v>
       </c>
       <c r="K68">
         <v>29</v>
@@ -22664,7 +22664,7 @@
         <v>130</v>
       </c>
       <c r="J69">
-        <v>74.115068489999999</v>
+        <v>74.099999999999994</v>
       </c>
       <c r="K69">
         <v>53</v>
@@ -22978,7 +22978,7 @@
         <v>130</v>
       </c>
       <c r="J70">
-        <v>77.095890409999996</v>
+        <v>77</v>
       </c>
       <c r="K70">
         <v>40</v>
@@ -23280,7 +23280,7 @@
         <v>116</v>
       </c>
       <c r="J71">
-        <v>52.309589039999999</v>
+        <v>52.3</v>
       </c>
       <c r="K71">
         <v>28</v>
@@ -23600,7 +23600,7 @@
         <v>130</v>
       </c>
       <c r="J72">
-        <v>57.890410959999997</v>
+        <v>57.8</v>
       </c>
       <c r="K72">
         <v>33</v>
@@ -23884,7 +23884,7 @@
         <v>130</v>
       </c>
       <c r="J73">
-        <v>70.868493150000006</v>
+        <v>70.8</v>
       </c>
       <c r="K73">
         <v>43</v>
@@ -24213,7 +24213,7 @@
         <v>130</v>
       </c>
       <c r="J74">
-        <v>46.306849319999998</v>
+        <v>46.3</v>
       </c>
       <c r="K74">
         <v>32</v>
@@ -24551,7 +24551,7 @@
         <v>130</v>
       </c>
       <c r="J75">
-        <v>60.383561640000003</v>
+        <v>60.3</v>
       </c>
       <c r="K75">
         <v>33</v>
@@ -24883,7 +24883,7 @@
         <v>130</v>
       </c>
       <c r="J76">
-        <v>50.443835620000002</v>
+        <v>50.4</v>
       </c>
       <c r="K76">
         <v>43</v>
@@ -25026,7 +25026,7 @@
         <v>116</v>
       </c>
       <c r="J77">
-        <v>70.972602739999999</v>
+        <v>70.900000000000006</v>
       </c>
       <c r="K77">
         <v>28</v>
@@ -25337,7 +25337,7 @@
         <v>116</v>
       </c>
       <c r="J78">
-        <v>61.534246580000001</v>
+        <v>61.5</v>
       </c>
       <c r="K78">
         <v>28</v>
@@ -25648,7 +25648,7 @@
         <v>116</v>
       </c>
       <c r="J79">
-        <v>67.238356159999995</v>
+        <v>67.2</v>
       </c>
       <c r="K79">
         <v>27</v>
@@ -25941,7 +25941,7 @@
         <v>116</v>
       </c>
       <c r="J80">
-        <v>51.578082190000003</v>
+        <v>51.5</v>
       </c>
       <c r="K80">
         <v>27</v>
@@ -26246,7 +26246,7 @@
         <v>116</v>
       </c>
       <c r="J81">
-        <v>50.317808220000003</v>
+        <v>50.3</v>
       </c>
       <c r="K81">
         <v>27</v>
@@ -26524,7 +26524,7 @@
         <v>116</v>
       </c>
       <c r="J82">
-        <v>64.679452049999995</v>
+        <v>64.599999999999994</v>
       </c>
       <c r="K82">
         <v>31</v>
@@ -26796,7 +26796,7 @@
         <v>116</v>
       </c>
       <c r="J83">
-        <v>59.189041099999997</v>
+        <v>59.1</v>
       </c>
       <c r="K83">
         <v>28</v>
@@ -27101,7 +27101,7 @@
         <v>116</v>
       </c>
       <c r="J84">
-        <v>65.46849315</v>
+        <v>65.400000000000006</v>
       </c>
       <c r="K84">
         <v>23</v>
@@ -27421,7 +27421,7 @@
         <v>116</v>
       </c>
       <c r="J85">
-        <v>54.2739726</v>
+        <v>54.2</v>
       </c>
       <c r="K85">
         <v>19</v>
@@ -27729,7 +27729,7 @@
         <v>116</v>
       </c>
       <c r="J86">
-        <v>69.950684929999994</v>
+        <v>69.900000000000006</v>
       </c>
       <c r="K86">
         <v>20</v>
@@ -28031,7 +28031,7 @@
         <v>116</v>
       </c>
       <c r="J87">
-        <v>64.126027399999998</v>
+        <v>64.099999999999994</v>
       </c>
       <c r="K87">
         <v>29</v>
@@ -28345,7 +28345,7 @@
         <v>116</v>
       </c>
       <c r="J88">
-        <v>59.783561640000002</v>
+        <v>59.7</v>
       </c>
       <c r="K88">
         <v>27</v>
@@ -28656,7 +28656,7 @@
         <v>116</v>
       </c>
       <c r="J89">
-        <v>38.413698629999999</v>
+        <v>38.4</v>
       </c>
       <c r="K89">
         <v>24</v>
@@ -28976,7 +28976,7 @@
         <v>116</v>
       </c>
       <c r="J90">
-        <v>30.63013699</v>
+        <v>30.6</v>
       </c>
       <c r="K90">
         <v>49</v>
@@ -29293,7 +29293,7 @@
         <v>116</v>
       </c>
       <c r="J91">
-        <v>58.15616438</v>
+        <v>58.1</v>
       </c>
       <c r="K91">
         <v>36</v>
@@ -29598,7 +29598,7 @@
         <v>116</v>
       </c>
       <c r="J92">
-        <v>66.663013699999993</v>
+        <v>66.599999999999994</v>
       </c>
       <c r="K92">
         <v>30</v>
@@ -29912,7 +29912,7 @@
         <v>116</v>
       </c>
       <c r="J93">
-        <v>65.084931510000004</v>
+        <v>65</v>
       </c>
       <c r="K93">
         <v>24</v>
@@ -30208,7 +30208,7 @@
         <v>116</v>
       </c>
       <c r="J94">
-        <v>57.435616439999997</v>
+        <v>57.4</v>
       </c>
       <c r="K94">
         <v>30</v>
@@ -30498,7 +30498,7 @@
         <v>116</v>
       </c>
       <c r="J95">
-        <v>56.668493150000003</v>
+        <v>56.6</v>
       </c>
       <c r="K95">
         <v>26</v>
@@ -30818,7 +30818,7 @@
         <v>116</v>
       </c>
       <c r="J96">
-        <v>39.942465749999997</v>
+        <v>39.9</v>
       </c>
       <c r="K96">
         <v>27</v>
@@ -31129,7 +31129,7 @@
         <v>116</v>
       </c>
       <c r="J97">
-        <v>56.690410960000001</v>
+        <v>56.6</v>
       </c>
       <c r="K97">
         <v>37</v>
@@ -31419,7 +31419,7 @@
         <v>116</v>
       </c>
       <c r="J98">
-        <v>62.19452055</v>
+        <v>62.1</v>
       </c>
       <c r="K98">
         <v>26</v>
@@ -31709,7 +31709,7 @@
         <v>116</v>
       </c>
       <c r="J99">
-        <v>62.263013700000002</v>
+        <v>62.2</v>
       </c>
       <c r="K99">
         <v>26</v>
@@ -32014,7 +32014,7 @@
         <v>116</v>
       </c>
       <c r="J100">
-        <v>69.501369859999997</v>
+        <v>69.5</v>
       </c>
       <c r="K100">
         <v>42</v>
@@ -32331,7 +32331,7 @@
         <v>116</v>
       </c>
       <c r="J101">
-        <v>73.950684929999994</v>
+        <v>73.900000000000006</v>
       </c>
       <c r="K101">
         <v>29</v>
@@ -32630,7 +32630,7 @@
         <v>116</v>
       </c>
       <c r="J102">
-        <v>67.53150685</v>
+        <v>67.5</v>
       </c>
       <c r="K102">
         <v>35</v>
@@ -32938,7 +32938,7 @@
         <v>116</v>
       </c>
       <c r="J103">
-        <v>57.268493149999998</v>
+        <v>57.2</v>
       </c>
       <c r="K103">
         <v>35</v>
@@ -33231,7 +33231,7 @@
         <v>116</v>
       </c>
       <c r="J104">
-        <v>64.53150685</v>
+        <v>64.5</v>
       </c>
       <c r="K104">
         <v>29</v>
@@ -33530,7 +33530,7 @@
         <v>116</v>
       </c>
       <c r="J105">
-        <v>47.797260270000002</v>
+        <v>47.7</v>
       </c>
       <c r="K105">
         <v>34</v>
@@ -33835,7 +33835,7 @@
         <v>116</v>
       </c>
       <c r="J106">
-        <v>32.117808220000001</v>
+        <v>32.1</v>
       </c>
       <c r="K106">
         <v>27</v>
@@ -34128,7 +34128,7 @@
         <v>116</v>
       </c>
       <c r="J107">
-        <v>68.227397260000004</v>
+        <v>68.2</v>
       </c>
       <c r="K107">
         <v>40</v>
@@ -34451,7 +34451,7 @@
         <v>116</v>
       </c>
       <c r="J108">
-        <v>66.632876710000005</v>
+        <v>66.599999999999994</v>
       </c>
       <c r="K108">
         <v>29</v>
@@ -34732,7 +34732,7 @@
         <v>116</v>
       </c>
       <c r="J109">
-        <v>34.019178080000003</v>
+        <v>34</v>
       </c>
       <c r="K109">
         <v>25</v>
@@ -35025,7 +35025,7 @@
         <v>116</v>
       </c>
       <c r="J110">
-        <v>34.509589040000002</v>
+        <v>34.5</v>
       </c>
       <c r="K110">
         <v>50</v>
@@ -35321,7 +35321,7 @@
         <v>116</v>
       </c>
       <c r="J111">
-        <v>79.430136989999994</v>
+        <v>79.400000000000006</v>
       </c>
       <c r="K111">
         <v>27</v>
@@ -35614,7 +35614,7 @@
         <v>116</v>
       </c>
       <c r="J112">
-        <v>49.769863010000002</v>
+        <v>49.7</v>
       </c>
       <c r="K112">
         <v>19</v>
@@ -35922,7 +35922,7 @@
         <v>116</v>
       </c>
       <c r="J113">
-        <v>65.126027399999998</v>
+        <v>65.099999999999994</v>
       </c>
       <c r="K113">
         <v>118</v>
@@ -36194,7 +36194,7 @@
         <v>116</v>
       </c>
       <c r="J114">
-        <v>25.728767120000001</v>
+        <v>25.7</v>
       </c>
       <c r="K114">
         <v>24</v>
@@ -36475,7 +36475,7 @@
         <v>116</v>
       </c>
       <c r="J115">
-        <v>63.46849315</v>
+        <v>63.4</v>
       </c>
       <c r="K115">
         <v>26</v>
@@ -36783,7 +36783,7 @@
         <v>116</v>
       </c>
       <c r="J116">
-        <v>41.030136990000003</v>
+        <v>41</v>
       </c>
       <c r="K116">
         <v>27</v>
@@ -37070,7 +37070,7 @@
         <v>116</v>
       </c>
       <c r="J117">
-        <v>64.758904110000003</v>
+        <v>64.7</v>
       </c>
       <c r="K117">
         <v>23</v>
@@ -37372,7 +37372,7 @@
         <v>116</v>
       </c>
       <c r="J118">
-        <v>67.328767119999995</v>
+        <v>67.3</v>
       </c>
       <c r="K118">
         <v>32</v>
@@ -37686,7 +37686,7 @@
         <v>116</v>
       </c>
       <c r="J119">
-        <v>68.054794520000002</v>
+        <v>68</v>
       </c>
       <c r="K119">
         <v>28</v>
@@ -37991,7 +37991,7 @@
         <v>116</v>
       </c>
       <c r="J120">
-        <v>63.769863010000002</v>
+        <v>63.7</v>
       </c>
       <c r="K120">
         <v>26</v>
@@ -38314,7 +38314,7 @@
         <v>116</v>
       </c>
       <c r="J121">
-        <v>65.632876710000005</v>
+        <v>65.599999999999994</v>
       </c>
       <c r="K121">
         <v>29</v>
@@ -38643,7 +38643,7 @@
         <v>116</v>
       </c>
       <c r="J122">
-        <v>76.753424659999993</v>
+        <v>76.7</v>
       </c>
       <c r="K122">
         <v>25</v>
@@ -38924,7 +38924,7 @@
         <v>116</v>
       </c>
       <c r="J123">
-        <v>49.019178080000003</v>
+        <v>49</v>
       </c>
       <c r="K123">
         <v>26</v>
@@ -39217,7 +39217,7 @@
         <v>116</v>
       </c>
       <c r="J124">
-        <v>61.216438359999998</v>
+        <v>61.2</v>
       </c>
       <c r="K124">
         <v>24</v>
@@ -39537,7 +39537,7 @@
         <v>116</v>
       </c>
       <c r="J125">
-        <v>73.550684930000003</v>
+        <v>73.5</v>
       </c>
       <c r="K125">
         <v>32</v>
@@ -39821,7 +39821,7 @@
         <v>116</v>
       </c>
       <c r="J126">
-        <v>68.802739729999999</v>
+        <v>68.8</v>
       </c>
       <c r="K126">
         <v>27</v>
@@ -40138,7 +40138,7 @@
         <v>116</v>
       </c>
       <c r="J127">
-        <v>67.572602739999994</v>
+        <v>67.5</v>
       </c>
       <c r="K127">
         <v>27</v>
@@ -40416,7 +40416,7 @@
         <v>116</v>
       </c>
       <c r="J128">
-        <v>58.29863014</v>
+        <v>58.2</v>
       </c>
       <c r="K128">
         <v>22</v>
@@ -40727,7 +40727,7 @@
         <v>116</v>
       </c>
       <c r="J129">
-        <v>76.534246580000001</v>
+        <v>76.5</v>
       </c>
       <c r="K129">
         <v>22</v>
@@ -41032,7 +41032,7 @@
         <v>116</v>
       </c>
       <c r="J130">
-        <v>63.641095890000003</v>
+        <v>63.6</v>
       </c>
       <c r="K130">
         <v>27</v>

</xml_diff>